<commit_message>
new example data with more variables
</commit_message>
<xml_diff>
--- a/data-raw/test_data.xlsx
+++ b/data-raw/test_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,6 +373,26 @@
           <t>altura</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>volumen_cc</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>diametro_rama</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>diametro_sc</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>biomasa_at</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -381,10 +401,22 @@
         </is>
       </c>
       <c r="B2">
-        <v>29.26050846938121</v>
+        <v>37.65470524253836</v>
       </c>
       <c r="C2">
-        <v>50.14310058725786</v>
+        <v>51.60811753977912</v>
+      </c>
+      <c r="D2">
+        <v>25.00457905980273</v>
+      </c>
+      <c r="E2">
+        <v>3.93912039008971</v>
+      </c>
+      <c r="F2">
+        <v>36.42790158405938</v>
+      </c>
+      <c r="G2">
+        <v>12.7006646585509</v>
       </c>
     </row>
     <row r="3">
@@ -394,10 +426,22 @@
         </is>
       </c>
       <c r="B3">
-        <v>34.8329717770122</v>
+        <v>20.97100979096255</v>
       </c>
       <c r="C3">
-        <v>51.09563379091706</v>
+        <v>46.74726622336478</v>
+      </c>
+      <c r="D3">
+        <v>20.35419253524632</v>
+      </c>
+      <c r="E3">
+        <v>4.570799538108062</v>
+      </c>
+      <c r="F3">
+        <v>20.09168406088467</v>
+      </c>
+      <c r="G3">
+        <v>12.21983402415254</v>
       </c>
     </row>
     <row r="4">
@@ -407,10 +451,22 @@
         </is>
       </c>
       <c r="B4">
-        <v>44.8981436772443</v>
+        <v>34.22435398320343</v>
       </c>
       <c r="C4">
-        <v>63.08278018132677</v>
+        <v>58.39944749847147</v>
+      </c>
+      <c r="D4">
+        <v>20.93177034923577</v>
+      </c>
+      <c r="E4">
+        <v>4.19193437285349</v>
+      </c>
+      <c r="F4">
+        <v>33.09469927288351</v>
+      </c>
+      <c r="G4">
+        <v>9.957154779937335</v>
       </c>
     </row>
     <row r="5">
@@ -420,10 +476,22 @@
         </is>
       </c>
       <c r="B5">
-        <v>26.13377473826234</v>
+        <v>27.01065832040039</v>
       </c>
       <c r="C5">
-        <v>60.19063694607349</v>
+        <v>57.19906017055213</v>
+      </c>
+      <c r="D5">
+        <v>26.80207719542889</v>
+      </c>
+      <c r="E5">
+        <v>4.167833153688601</v>
+      </c>
+      <c r="F5">
+        <v>26.12571691850498</v>
+      </c>
+      <c r="G5">
+        <v>12.42942274984988</v>
       </c>
     </row>
     <row r="6">
@@ -433,10 +501,22 @@
         </is>
       </c>
       <c r="B6">
-        <v>47.3170993518597</v>
+        <v>30.30809353197209</v>
       </c>
       <c r="C6">
-        <v>60.62056638552377</v>
+        <v>50.43318139233984</v>
+      </c>
+      <c r="D6">
+        <v>18.60766475266841</v>
+      </c>
+      <c r="E6">
+        <v>4.337089993462782</v>
+      </c>
+      <c r="F6">
+        <v>29.37932523827054</v>
+      </c>
+      <c r="G6">
+        <v>11.34684901803972</v>
       </c>
     </row>
     <row r="7">
@@ -446,10 +526,22 @@
         </is>
       </c>
       <c r="B7">
-        <v>25.72469126066345</v>
+        <v>37.86030076638916</v>
       </c>
       <c r="C7">
-        <v>65.56690472447228</v>
+        <v>50.13882879230731</v>
+      </c>
+      <c r="D7">
+        <v>20.75980616959321</v>
+      </c>
+      <c r="E7">
+        <v>4.056559841534987</v>
+      </c>
+      <c r="F7">
+        <v>36.56995871114724</v>
+      </c>
+      <c r="G7">
+        <v>11.01896954294679</v>
       </c>
     </row>
     <row r="8">
@@ -459,10 +551,22 @@
         </is>
       </c>
       <c r="B8">
-        <v>25.51571929055174</v>
+        <v>17.41162252061773</v>
       </c>
       <c r="C8">
-        <v>66.95469550797006</v>
+        <v>57.82461120784519</v>
+      </c>
+      <c r="D8">
+        <v>21.12503409202439</v>
+      </c>
+      <c r="E8">
+        <v>4.007577704510279</v>
+      </c>
+      <c r="F8">
+        <v>16.363738553627</v>
+      </c>
+      <c r="G8">
+        <v>11.18789447720029</v>
       </c>
     </row>
     <row r="9">
@@ -472,10 +576,22 @@
         </is>
       </c>
       <c r="B9">
-        <v>38.02451422237979</v>
+        <v>29.90603410714481</v>
       </c>
       <c r="C9">
-        <v>43.39649299245033</v>
+        <v>60.22557999494267</v>
+      </c>
+      <c r="D9">
+        <v>22.40846067416646</v>
+      </c>
+      <c r="E9">
+        <v>3.89469386324063</v>
+      </c>
+      <c r="F9">
+        <v>28.52566574501708</v>
+      </c>
+      <c r="G9">
+        <v>12.68680548806134</v>
       </c>
     </row>
     <row r="10">
@@ -485,10 +601,22 @@
         </is>
       </c>
       <c r="B10">
-        <v>43.03101603162236</v>
+        <v>33.6708536881677</v>
       </c>
       <c r="C10">
-        <v>52.98236772410904</v>
+        <v>55.57361178643664</v>
+      </c>
+      <c r="D10">
+        <v>24.78012766868317</v>
+      </c>
+      <c r="E10">
+        <v>3.969889516805412</v>
+      </c>
+      <c r="F10">
+        <v>32.54157885238983</v>
+      </c>
+      <c r="G10">
+        <v>10.89808268479217</v>
       </c>
     </row>
     <row r="11">
@@ -498,10 +626,22 @@
         </is>
       </c>
       <c r="B11">
-        <v>31.84047173610129</v>
+        <v>39.85013860962474</v>
       </c>
       <c r="C11">
-        <v>50.13597000812062</v>
+        <v>43.39342116480934</v>
+      </c>
+      <c r="D11">
+        <v>18.87339386103286</v>
+      </c>
+      <c r="E11">
+        <v>4.064821503611319</v>
+      </c>
+      <c r="F11">
+        <v>38.7274428145985</v>
+      </c>
+      <c r="G11">
+        <v>11.82099995734923</v>
       </c>
     </row>
     <row r="12">
@@ -511,10 +651,22 @@
         </is>
       </c>
       <c r="B12">
-        <v>30.61118711730373</v>
+        <v>32.92344918358401</v>
       </c>
       <c r="C12">
-        <v>62.06576402270056</v>
+        <v>56.73362444618044</v>
+      </c>
+      <c r="D12">
+        <v>20.93326450150323</v>
+      </c>
+      <c r="E12">
+        <v>3.672583864653439</v>
+      </c>
+      <c r="F12">
+        <v>31.91037127876553</v>
+      </c>
+      <c r="G12">
+        <v>12.20199824644098</v>
       </c>
     </row>
     <row r="13">
@@ -524,10 +676,22 @@
         </is>
       </c>
       <c r="B13">
-        <v>18.8706509122467</v>
+        <v>34.24266009634698</v>
       </c>
       <c r="C13">
-        <v>57.42823027472692</v>
+        <v>63.67588050353686</v>
+      </c>
+      <c r="D13">
+        <v>20.23771070391746</v>
+      </c>
+      <c r="E13">
+        <v>4.043443656483573</v>
+      </c>
+      <c r="F13">
+        <v>33.19268022034263</v>
+      </c>
+      <c r="G13">
+        <v>11.27805053632479</v>
       </c>
     </row>
     <row r="14">
@@ -537,10 +701,22 @@
         </is>
       </c>
       <c r="B14">
-        <v>30.18425279591796</v>
+        <v>30.94719643581384</v>
       </c>
       <c r="C14">
-        <v>54.76749037053637</v>
+        <v>66.45184322966156</v>
+      </c>
+      <c r="D14">
+        <v>26.003565058598</v>
+      </c>
+      <c r="E14">
+        <v>3.637028880890962</v>
+      </c>
+      <c r="F14">
+        <v>29.88821970697106</v>
+      </c>
+      <c r="G14">
+        <v>10.72476988564182</v>
       </c>
     </row>
     <row r="15">
@@ -550,10 +726,22 @@
         </is>
       </c>
       <c r="B15">
-        <v>20.95331850584069</v>
+        <v>44.54115198951872</v>
       </c>
       <c r="C15">
-        <v>53.95565452278879</v>
+        <v>63.04675453529266</v>
+      </c>
+      <c r="D15">
+        <v>20.8792417725417</v>
+      </c>
+      <c r="E15">
+        <v>3.852835884805435</v>
+      </c>
+      <c r="F15">
+        <v>43.48884352608171</v>
+      </c>
+      <c r="G15">
+        <v>12.37514250767625</v>
       </c>
     </row>
     <row r="16">
@@ -563,10 +751,22 @@
         </is>
       </c>
       <c r="B16">
-        <v>26.48072698292131</v>
+        <v>24.06855948549612</v>
       </c>
       <c r="C16">
-        <v>58.85403083157869</v>
+        <v>59.21441381213636</v>
+      </c>
+      <c r="D16">
+        <v>23.17662940860284</v>
+      </c>
+      <c r="E16">
+        <v>4.088447966667184</v>
+      </c>
+      <c r="F16">
+        <v>23.08816139437155</v>
+      </c>
+      <c r="G16">
+        <v>11.47829877636936</v>
       </c>
     </row>
     <row r="17">
@@ -576,10 +776,22 @@
         </is>
       </c>
       <c r="B17">
-        <v>34.31695093262816</v>
+        <v>37.72137845966181</v>
       </c>
       <c r="C17">
-        <v>58.92853833168409</v>
+        <v>43.62744567770756</v>
+      </c>
+      <c r="D17">
+        <v>17.78133618632105</v>
+      </c>
+      <c r="E17">
+        <v>3.72562727713383</v>
+      </c>
+      <c r="F17">
+        <v>36.38599662484617</v>
+      </c>
+      <c r="G17">
+        <v>12.15563143427057</v>
       </c>
     </row>
     <row r="18">
@@ -589,10 +801,22 @@
         </is>
       </c>
       <c r="B18">
-        <v>27.75808752594851</v>
+        <v>21.62365894776661</v>
       </c>
       <c r="C18">
-        <v>49.37100820861512</v>
+        <v>46.58975662188578</v>
+      </c>
+      <c r="D18">
+        <v>19.41548606929283</v>
+      </c>
+      <c r="E18">
+        <v>4.190839244644159</v>
+      </c>
+      <c r="F18">
+        <v>20.5560441912471</v>
+      </c>
+      <c r="G18">
+        <v>11.89111167611359</v>
       </c>
     </row>
     <row r="19">
@@ -602,10 +826,22 @@
         </is>
       </c>
       <c r="B19">
-        <v>30.93226754896128</v>
+        <v>33.76405103089152</v>
       </c>
       <c r="C19">
-        <v>67.69714756567308</v>
+        <v>59.94114649615088</v>
+      </c>
+      <c r="D19">
+        <v>25.08524639721132</v>
+      </c>
+      <c r="E19">
+        <v>4.457637275158071</v>
+      </c>
+      <c r="F19">
+        <v>32.96555042034831</v>
+      </c>
+      <c r="G19">
+        <v>11.7360884031035</v>
       </c>
     </row>
     <row r="20">
@@ -615,10 +851,22 @@
         </is>
       </c>
       <c r="B20">
-        <v>31.46477997016459</v>
+        <v>40.28132837342843</v>
       </c>
       <c r="C20">
-        <v>55.02966351900832</v>
+        <v>52.6318227536204</v>
+      </c>
+      <c r="D20">
+        <v>21.64971347213327</v>
+      </c>
+      <c r="E20">
+        <v>3.882515394166306</v>
+      </c>
+      <c r="F20">
+        <v>39.27228495843555</v>
+      </c>
+      <c r="G20">
+        <v>11.07877164147892</v>
       </c>
     </row>
     <row r="21">
@@ -628,10 +876,22 @@
         </is>
       </c>
       <c r="B21">
-        <v>44.20089604239213</v>
+        <v>21.18051572518408</v>
       </c>
       <c r="C21">
-        <v>45.74563913124314</v>
+        <v>66.06121547558527</v>
+      </c>
+      <c r="D21">
+        <v>29.0845391083618</v>
+      </c>
+      <c r="E21">
+        <v>4.124588633871171</v>
+      </c>
+      <c r="F21">
+        <v>19.96473657934687</v>
+      </c>
+      <c r="G21">
+        <v>11.96315291045</v>
       </c>
     </row>
     <row r="22">
@@ -641,10 +901,22 @@
         </is>
       </c>
       <c r="B22">
-        <v>21.36253619188613</v>
+        <v>31.421385105193</v>
       </c>
       <c r="C22">
-        <v>72.44023460460532</v>
+        <v>62.25280095220126</v>
+      </c>
+      <c r="D22">
+        <v>24.64637549244251</v>
+      </c>
+      <c r="E22">
+        <v>3.731283441681519</v>
+      </c>
+      <c r="F22">
+        <v>30.55863162917073</v>
+      </c>
+      <c r="G22">
+        <v>15.40220834773072</v>
       </c>
     </row>
     <row r="23">
@@ -654,10 +926,22 @@
         </is>
       </c>
       <c r="B23">
-        <v>34.65124635091045</v>
+        <v>36.34682896488388</v>
       </c>
       <c r="C23">
-        <v>64.21977124451398</v>
+        <v>36.17025408849867</v>
+      </c>
+      <c r="D23">
+        <v>21.43543427273226</v>
+      </c>
+      <c r="E23">
+        <v>3.925586315956076</v>
+      </c>
+      <c r="F23">
+        <v>35.21920066111527</v>
+      </c>
+      <c r="G23">
+        <v>11.23008743280924</v>
       </c>
     </row>
     <row r="24">
@@ -667,10 +951,22 @@
         </is>
       </c>
       <c r="B24">
-        <v>32.33860143828026</v>
+        <v>31.97005672068734</v>
       </c>
       <c r="C24">
-        <v>61.95371694614136</v>
+        <v>56.27796839443388</v>
+      </c>
+      <c r="D24">
+        <v>21.88359965327338</v>
+      </c>
+      <c r="E24">
+        <v>4.0343376878975</v>
+      </c>
+      <c r="F24">
+        <v>31.14495476430598</v>
+      </c>
+      <c r="G24">
+        <v>11.00933853716675</v>
       </c>
     </row>
     <row r="25">
@@ -680,10 +976,22 @@
         </is>
       </c>
       <c r="B25">
-        <v>45.56735386470822</v>
+        <v>25.94710316689102</v>
       </c>
       <c r="C25">
-        <v>56.73238648633686</v>
+        <v>50.97168467636153</v>
+      </c>
+      <c r="D25">
+        <v>19.62150266538104</v>
+      </c>
+      <c r="E25">
+        <v>4.013413248467549</v>
+      </c>
+      <c r="F25">
+        <v>25.09629582291078</v>
+      </c>
+      <c r="G25">
+        <v>12.35357432409563</v>
       </c>
     </row>
     <row r="26">
@@ -693,10 +1001,22 @@
         </is>
       </c>
       <c r="B26">
-        <v>22.63108784643516</v>
+        <v>29.07641995977397</v>
       </c>
       <c r="C26">
-        <v>52.03965671303396</v>
+        <v>55.6439078461252</v>
+      </c>
+      <c r="D26">
+        <v>22.23924967144885</v>
+      </c>
+      <c r="E26">
+        <v>4.186162613982727</v>
+      </c>
+      <c r="F26">
+        <v>27.823645545369</v>
+      </c>
+      <c r="G26">
+        <v>12.01654744336551</v>
       </c>
     </row>
     <row r="27">
@@ -706,10 +1026,22 @@
         </is>
       </c>
       <c r="B27">
-        <v>26.59444631087039</v>
+        <v>38.66968168200144</v>
       </c>
       <c r="C27">
-        <v>54.82791297576725</v>
+        <v>46.66762768733577</v>
+      </c>
+      <c r="D27">
+        <v>23.33421677317942</v>
+      </c>
+      <c r="E27">
+        <v>3.939564058556785</v>
+      </c>
+      <c r="F27">
+        <v>37.75004567172401</v>
+      </c>
+      <c r="G27">
+        <v>12.51709427836907</v>
       </c>
     </row>
     <row r="28">
@@ -719,10 +1051,22 @@
         </is>
       </c>
       <c r="B28">
-        <v>27.8858960733983</v>
+        <v>28.31303375318503</v>
       </c>
       <c r="C28">
-        <v>58.93008450529034</v>
+        <v>53.18859161155486</v>
+      </c>
+      <c r="D28">
+        <v>25.39000807269398</v>
+      </c>
+      <c r="E28">
+        <v>4.003620703225296</v>
+      </c>
+      <c r="F28">
+        <v>27.34839929557971</v>
+      </c>
+      <c r="G28">
+        <v>10.22115853083084</v>
       </c>
     </row>
     <row r="29">
@@ -732,10 +1076,22 @@
         </is>
       </c>
       <c r="B29">
-        <v>41.81603686414086</v>
+        <v>30.0506799868974</v>
       </c>
       <c r="C29">
-        <v>51.87606615267571</v>
+        <v>73.61892362130112</v>
+      </c>
+      <c r="D29">
+        <v>21.94451929467446</v>
+      </c>
+      <c r="E29">
+        <v>4.110113155542677</v>
+      </c>
+      <c r="F29">
+        <v>28.82794491978407</v>
+      </c>
+      <c r="G29">
+        <v>10.60906999296019</v>
       </c>
     </row>
     <row r="30">
@@ -745,10 +1101,22 @@
         </is>
       </c>
       <c r="B30">
-        <v>18.74104922342048</v>
+        <v>41.01876170546831</v>
       </c>
       <c r="C30">
-        <v>65.61932000289389</v>
+        <v>49.07755539845868</v>
+      </c>
+      <c r="D30">
+        <v>24.02579960502164</v>
+      </c>
+      <c r="E30">
+        <v>3.920760644064361</v>
+      </c>
+      <c r="F30">
+        <v>39.88227126359697</v>
+      </c>
+      <c r="G30">
+        <v>12.79346384069571</v>
       </c>
     </row>
     <row r="31">
@@ -758,10 +1126,22 @@
         </is>
       </c>
       <c r="B31">
-        <v>29.95842136105826</v>
+        <v>39.02577134033249</v>
       </c>
       <c r="C31">
-        <v>55.69977376752747</v>
+        <v>61.39452056826808</v>
+      </c>
+      <c r="D31">
+        <v>21.72498023665119</v>
+      </c>
+      <c r="E31">
+        <v>4.044764808858409</v>
+      </c>
+      <c r="F31">
+        <v>38.42748851480467</v>
+      </c>
+      <c r="G31">
+        <v>11.2589450943231</v>
       </c>
     </row>
     <row r="32">
@@ -771,10 +1151,22 @@
         </is>
       </c>
       <c r="B32">
-        <v>32.78122991429154</v>
+        <v>38.68473792450907</v>
       </c>
       <c r="C32">
-        <v>51.75323821742613</v>
+        <v>49.91440346432987</v>
+      </c>
+      <c r="D32">
+        <v>21.70039671584801</v>
+      </c>
+      <c r="E32">
+        <v>3.987685026343994</v>
+      </c>
+      <c r="F32">
+        <v>37.60456839641626</v>
+      </c>
+      <c r="G32">
+        <v>10.79082674154445</v>
       </c>
     </row>
     <row r="33">
@@ -784,10 +1176,22 @@
         </is>
       </c>
       <c r="B33">
-        <v>22.22537494668633</v>
+        <v>46.60609466536783</v>
       </c>
       <c r="C33">
-        <v>54.43762487824615</v>
+        <v>62.63787235140653</v>
+      </c>
+      <c r="D33">
+        <v>24.0745868530753</v>
+      </c>
+      <c r="E33">
+        <v>4.236109495761594</v>
+      </c>
+      <c r="F33">
+        <v>45.67293807146485</v>
+      </c>
+      <c r="G33">
+        <v>11.02820431376807</v>
       </c>
     </row>
     <row r="34">
@@ -797,10 +1201,22 @@
         </is>
       </c>
       <c r="B34">
-        <v>37.72487393354207</v>
+        <v>15.49124084464814</v>
       </c>
       <c r="C34">
-        <v>50.79168378863609</v>
+        <v>58.08981486503161</v>
+      </c>
+      <c r="D34">
+        <v>21.0887957565587</v>
+      </c>
+      <c r="E34">
+        <v>3.648694543917573</v>
+      </c>
+      <c r="F34">
+        <v>14.57564171772989</v>
+      </c>
+      <c r="G34">
+        <v>13.3732648263251</v>
       </c>
     </row>
     <row r="35">
@@ -810,10 +1226,22 @@
         </is>
       </c>
       <c r="B35">
-        <v>25.94239598877775</v>
+        <v>31.53267773223707</v>
       </c>
       <c r="C35">
-        <v>55.33252172299959</v>
+        <v>65.03273663109069</v>
+      </c>
+      <c r="D35">
+        <v>24.80549644653609</v>
+      </c>
+      <c r="E35">
+        <v>4.518532575470232</v>
+      </c>
+      <c r="F35">
+        <v>30.94179644543985</v>
+      </c>
+      <c r="G35">
+        <v>10.16108130811879</v>
       </c>
     </row>
     <row r="36">
@@ -823,10 +1251,22 @@
         </is>
       </c>
       <c r="B36">
-        <v>31.81017088011442</v>
+        <v>33.63412735250948</v>
       </c>
       <c r="C36">
-        <v>48.97850483174109</v>
+        <v>45.3223707933924</v>
+      </c>
+      <c r="D36">
+        <v>18.89531374268416</v>
+      </c>
+      <c r="E36">
+        <v>3.790911818129372</v>
+      </c>
+      <c r="F36">
+        <v>32.53809783231152</v>
+      </c>
+      <c r="G36">
+        <v>12.82090276793567</v>
       </c>
     </row>
     <row r="37">
@@ -836,10 +1276,22 @@
         </is>
       </c>
       <c r="B37">
-        <v>26.84170155884106</v>
+        <v>40.22925429150636</v>
       </c>
       <c r="C37">
-        <v>55.12339214198921</v>
+        <v>51.59737710416096</v>
+      </c>
+      <c r="D37">
+        <v>24.64350047580776</v>
+      </c>
+      <c r="E37">
+        <v>4.211179257673479</v>
+      </c>
+      <c r="F37">
+        <v>38.81430777276957</v>
+      </c>
+      <c r="G37">
+        <v>13.28081746631205</v>
       </c>
     </row>
     <row r="38">
@@ -849,10 +1301,22 @@
         </is>
       </c>
       <c r="B38">
-        <v>36.37938117850533</v>
+        <v>40.03237072697644</v>
       </c>
       <c r="C38">
-        <v>42.22179565814439</v>
+        <v>54.50127256775549</v>
+      </c>
+      <c r="D38">
+        <v>23.14418486505264</v>
+      </c>
+      <c r="E38">
+        <v>3.717336759489281</v>
+      </c>
+      <c r="F38">
+        <v>38.96273175405387</v>
+      </c>
+      <c r="G38">
+        <v>10.2505319624795</v>
       </c>
     </row>
     <row r="39">
@@ -862,10 +1326,22 @@
         </is>
       </c>
       <c r="B39">
-        <v>33.08261328414495</v>
+        <v>38.70433357256674</v>
       </c>
       <c r="C39">
-        <v>55.74070710191165</v>
+        <v>45.65553791039255</v>
+      </c>
+      <c r="D39">
+        <v>25.32428293874744</v>
+      </c>
+      <c r="E39">
+        <v>4.036605343208179</v>
+      </c>
+      <c r="F39">
+        <v>37.71835298240355</v>
+      </c>
+      <c r="G39">
+        <v>12.86876532496196</v>
       </c>
     </row>
     <row r="40">
@@ -875,10 +1351,22 @@
         </is>
       </c>
       <c r="B40">
-        <v>31.9710942372681</v>
+        <v>37.04141998764807</v>
       </c>
       <c r="C40">
-        <v>45.76882295617047</v>
+        <v>60.08710566012363</v>
+      </c>
+      <c r="D40">
+        <v>23.78945179515889</v>
+      </c>
+      <c r="E40">
+        <v>3.954469681961223</v>
+      </c>
+      <c r="F40">
+        <v>35.88998744336345</v>
+      </c>
+      <c r="G40">
+        <v>16.28133318413483</v>
       </c>
     </row>
     <row r="41">
@@ -888,10 +1376,22 @@
         </is>
       </c>
       <c r="B41">
-        <v>48.51669264068822</v>
+        <v>39.55848816951026</v>
       </c>
       <c r="C41">
-        <v>52.24692126452273</v>
+        <v>53.7124260766635</v>
+      </c>
+      <c r="D41">
+        <v>25.14249211316371</v>
+      </c>
+      <c r="E41">
+        <v>3.780313752462677</v>
+      </c>
+      <c r="F41">
+        <v>38.29847949242452</v>
+      </c>
+      <c r="G41">
+        <v>11.17958634459797</v>
       </c>
     </row>
     <row r="42">
@@ -901,10 +1401,22 @@
         </is>
       </c>
       <c r="B42">
-        <v>32.32172280965622</v>
+        <v>18.29604667046423</v>
       </c>
       <c r="C42">
-        <v>54.18687533199584</v>
+        <v>53.12707673658984</v>
+      </c>
+      <c r="D42">
+        <v>23.78039256161029</v>
+      </c>
+      <c r="E42">
+        <v>4.040360189179484</v>
+      </c>
+      <c r="F42">
+        <v>16.97176326888339</v>
+      </c>
+      <c r="G42">
+        <v>13.94481095893269</v>
       </c>
     </row>
     <row r="43">
@@ -914,10 +1426,22 @@
         </is>
       </c>
       <c r="B43">
-        <v>25.02939720018023</v>
+        <v>23.65829815727003</v>
       </c>
       <c r="C43">
-        <v>46.68602705826856</v>
+        <v>62.23016035680324</v>
+      </c>
+      <c r="D43">
+        <v>24.1060579548981</v>
+      </c>
+      <c r="E43">
+        <v>3.966855785286509</v>
+      </c>
+      <c r="F43">
+        <v>22.65380321008976</v>
+      </c>
+      <c r="G43">
+        <v>12.98936170540462</v>
       </c>
     </row>
     <row r="44">
@@ -927,10 +1451,22 @@
         </is>
       </c>
       <c r="B44">
-        <v>36.16749585281678</v>
+        <v>27.29571929464089</v>
       </c>
       <c r="C44">
-        <v>52.62938548680582</v>
+        <v>63.37458098050345</v>
+      </c>
+      <c r="D44">
+        <v>21.65907228763496</v>
+      </c>
+      <c r="E44">
+        <v>4.051855091742398</v>
+      </c>
+      <c r="F44">
+        <v>26.39124639605577</v>
+      </c>
+      <c r="G44">
+        <v>11.20426183116647</v>
       </c>
     </row>
     <row r="45">
@@ -940,10 +1476,22 @@
         </is>
       </c>
       <c r="B45">
-        <v>26.25201366544255</v>
+        <v>36.15153890171119</v>
       </c>
       <c r="C45">
-        <v>78.11584944586298</v>
+        <v>58.81445433463105</v>
+      </c>
+      <c r="D45">
+        <v>26.20104079434911</v>
+      </c>
+      <c r="E45">
+        <v>4.056309442120025</v>
+      </c>
+      <c r="F45">
+        <v>35.38493114005701</v>
+      </c>
+      <c r="G45">
+        <v>11.26379776340742</v>
       </c>
     </row>
     <row r="46">
@@ -953,10 +1501,22 @@
         </is>
       </c>
       <c r="B46">
-        <v>20.44137142819425</v>
+        <v>19.22139842559059</v>
       </c>
       <c r="C46">
-        <v>57.05219607892651</v>
+        <v>62.05920836063404</v>
+      </c>
+      <c r="D46">
+        <v>26.13169229143967</v>
+      </c>
+      <c r="E46">
+        <v>3.885240201419369</v>
+      </c>
+      <c r="F46">
+        <v>18.28828955860348</v>
+      </c>
+      <c r="G46">
+        <v>11.48817815678689</v>
       </c>
     </row>
     <row r="47">
@@ -966,10 +1526,22 @@
         </is>
       </c>
       <c r="B47">
-        <v>39.88520678913323</v>
+        <v>32.83157805346922</v>
       </c>
       <c r="C47">
-        <v>37.26772451238292</v>
+        <v>71.20800035329958</v>
+      </c>
+      <c r="D47">
+        <v>23.88787246383341</v>
+      </c>
+      <c r="E47">
+        <v>3.959037633777772</v>
+      </c>
+      <c r="F47">
+        <v>32.00352914538298</v>
+      </c>
+      <c r="G47">
+        <v>10.95662294759684</v>
       </c>
     </row>
     <row r="48">
@@ -979,10 +1551,22 @@
         </is>
       </c>
       <c r="B48">
-        <v>37.50981365772365</v>
+        <v>28.69149627074416</v>
       </c>
       <c r="C48">
-        <v>56.04194453545513</v>
+        <v>59.00612895211994</v>
+      </c>
+      <c r="D48">
+        <v>22.19294409080805</v>
+      </c>
+      <c r="E48">
+        <v>3.956991634733434</v>
+      </c>
+      <c r="F48">
+        <v>27.49442192655647</v>
+      </c>
+      <c r="G48">
+        <v>12.49258149389427</v>
       </c>
     </row>
     <row r="49">
@@ -992,10 +1576,22 @@
         </is>
       </c>
       <c r="B49">
-        <v>36.80636680873391</v>
+        <v>25.86158880974735</v>
       </c>
       <c r="C49">
-        <v>50.04209762281565</v>
+        <v>51.65321541048667</v>
+      </c>
+      <c r="D49">
+        <v>24.71032863718846</v>
+      </c>
+      <c r="E49">
+        <v>3.879281084518345</v>
+      </c>
+      <c r="F49">
+        <v>24.98540757350582</v>
+      </c>
+      <c r="G49">
+        <v>12.59048968284478</v>
       </c>
     </row>
     <row r="50">
@@ -1005,10 +1601,22 @@
         </is>
       </c>
       <c r="B50">
-        <v>45.3572099985585</v>
+        <v>35.15391608446489</v>
       </c>
       <c r="C50">
-        <v>70.84128184014986</v>
+        <v>60.88243532413802</v>
+      </c>
+      <c r="D50">
+        <v>24.72188633904995</v>
+      </c>
+      <c r="E50">
+        <v>3.839001528078542</v>
+      </c>
+      <c r="F50">
+        <v>34.44010167640275</v>
+      </c>
+      <c r="G50">
+        <v>11.19419998509121</v>
       </c>
     </row>
     <row r="51">
@@ -1018,10 +1626,22 @@
         </is>
       </c>
       <c r="B51">
-        <v>31.52654749136752</v>
+        <v>27.40591888597443</v>
       </c>
       <c r="C51">
-        <v>53.85177928160606</v>
+        <v>63.30628363311063</v>
+      </c>
+      <c r="D51">
+        <v>19.56200289641962</v>
+      </c>
+      <c r="E51">
+        <v>4.04576793708875</v>
+      </c>
+      <c r="F51">
+        <v>26.30668280092452</v>
+      </c>
+      <c r="G51">
+        <v>11.30734199476279</v>
       </c>
     </row>
     <row r="52">
@@ -1031,10 +1651,22 @@
         </is>
       </c>
       <c r="B52">
-        <v>26.761249603769</v>
+        <v>18.79758837750188</v>
       </c>
       <c r="C52">
-        <v>44.90537917492502</v>
+        <v>60.32043883000523</v>
+      </c>
+      <c r="D52">
+        <v>25.67078326735856</v>
+      </c>
+      <c r="E52">
+        <v>4.007126724071537</v>
+      </c>
+      <c r="F52">
+        <v>17.95148693540467</v>
+      </c>
+      <c r="G52">
+        <v>12.78736794813037</v>
       </c>
     </row>
     <row r="53">
@@ -1044,10 +1676,22 @@
         </is>
       </c>
       <c r="B53">
-        <v>37.67071126525349</v>
+        <v>47.31442133581969</v>
       </c>
       <c r="C53">
-        <v>60.33021457605118</v>
+        <v>52.46172700927396</v>
+      </c>
+      <c r="D53">
+        <v>23.59348066100358</v>
+      </c>
+      <c r="E53">
+        <v>3.824330791336362</v>
+      </c>
+      <c r="F53">
+        <v>46.36698746392701</v>
+      </c>
+      <c r="G53">
+        <v>12.11976177749385</v>
       </c>
     </row>
     <row r="54">
@@ -1057,10 +1701,22 @@
         </is>
       </c>
       <c r="B54">
-        <v>18.24543944763956</v>
+        <v>32.8134299473178</v>
       </c>
       <c r="C54">
-        <v>41.77917381706023</v>
+        <v>61.71831746079372</v>
+      </c>
+      <c r="D54">
+        <v>23.78455667943076</v>
+      </c>
+      <c r="E54">
+        <v>3.677021801709767</v>
+      </c>
+      <c r="F54">
+        <v>31.87098122807645</v>
+      </c>
+      <c r="G54">
+        <v>10.04601424065373</v>
       </c>
     </row>
     <row r="55">
@@ -1070,10 +1726,22 @@
         </is>
       </c>
       <c r="B55">
-        <v>31.72862424761231</v>
+        <v>13.69001882927202</v>
       </c>
       <c r="C55">
-        <v>53.78577589523695</v>
+        <v>52.97839432629816</v>
+      </c>
+      <c r="D55">
+        <v>20.21500537865302</v>
+      </c>
+      <c r="E55">
+        <v>4.164825497596795</v>
+      </c>
+      <c r="F55">
+        <v>12.71006130055792</v>
+      </c>
+      <c r="G55">
+        <v>11.74113189189027</v>
       </c>
     </row>
     <row r="56">
@@ -1083,10 +1751,22 @@
         </is>
       </c>
       <c r="B56">
-        <v>30.92479923315897</v>
+        <v>38.43083077281985</v>
       </c>
       <c r="C56">
-        <v>44.6772419636637</v>
+        <v>54.07181034015292</v>
+      </c>
+      <c r="D56">
+        <v>29.77048365489942</v>
+      </c>
+      <c r="E56">
+        <v>4.118590948182908</v>
+      </c>
+      <c r="F56">
+        <v>37.34924602659681</v>
+      </c>
+      <c r="G56">
+        <v>11.3086059330984</v>
       </c>
     </row>
     <row r="57">
@@ -1096,10 +1776,22 @@
         </is>
       </c>
       <c r="B57">
-        <v>25.99773102449686</v>
+        <v>30.35170624910084</v>
       </c>
       <c r="C57">
-        <v>66.97694912650211</v>
+        <v>50.97305146235153</v>
+      </c>
+      <c r="D57">
+        <v>22.92876440444298</v>
+      </c>
+      <c r="E57">
+        <v>4.386820346122387</v>
+      </c>
+      <c r="F57">
+        <v>29.22428051428354</v>
+      </c>
+      <c r="G57">
+        <v>12.8712865826213</v>
       </c>
     </row>
     <row r="58">
@@ -1109,10 +1801,22 @@
         </is>
       </c>
       <c r="B58">
-        <v>36.55539701156378</v>
+        <v>14.46076939382364</v>
       </c>
       <c r="C58">
-        <v>54.83667239186472</v>
+        <v>56.66702010251574</v>
+      </c>
+      <c r="D58">
+        <v>21.48893451398033</v>
+      </c>
+      <c r="E58">
+        <v>4.103078507433067</v>
+      </c>
+      <c r="F58">
+        <v>13.56588560519194</v>
+      </c>
+      <c r="G58">
+        <v>11.23653688208632</v>
       </c>
     </row>
     <row r="59">
@@ -1122,10 +1826,22 @@
         </is>
       </c>
       <c r="B59">
-        <v>34.80732474586311</v>
+        <v>36.81778694521051</v>
       </c>
       <c r="C59">
-        <v>51.93457659157027</v>
+        <v>43.42971522695744</v>
+      </c>
+      <c r="D59">
+        <v>22.48912349407896</v>
+      </c>
+      <c r="E59">
+        <v>3.978045150786237</v>
+      </c>
+      <c r="F59">
+        <v>35.8959323635406</v>
+      </c>
+      <c r="G59">
+        <v>12.00619455119</v>
       </c>
     </row>
     <row r="60">
@@ -1135,10 +1851,22 @@
         </is>
       </c>
       <c r="B60">
-        <v>26.39873904448391</v>
+        <v>37.92944268600351</v>
       </c>
       <c r="C60">
-        <v>42.47397651620724</v>
+        <v>58.77774346657601</v>
+      </c>
+      <c r="D60">
+        <v>21.32782632785393</v>
+      </c>
+      <c r="E60">
+        <v>3.809307714987126</v>
+      </c>
+      <c r="F60">
+        <v>37.09940890698135</v>
+      </c>
+      <c r="G60">
+        <v>9.996772009541274</v>
       </c>
     </row>
     <row r="61">
@@ -1148,10 +1876,22 @@
         </is>
       </c>
       <c r="B61">
-        <v>47.36226994740582</v>
+        <v>42.70749231885191</v>
       </c>
       <c r="C61">
-        <v>65.68576935910555</v>
+        <v>56.90753173971254</v>
+      </c>
+      <c r="D61">
+        <v>22.86824910695478</v>
+      </c>
+      <c r="E61">
+        <v>4.090656264108995</v>
+      </c>
+      <c r="F61">
+        <v>41.58823658568825</v>
+      </c>
+      <c r="G61">
+        <v>11.64372938004363</v>
       </c>
     </row>
     <row r="62">
@@ -1161,10 +1901,22 @@
         </is>
       </c>
       <c r="B62">
-        <v>34.75115070216967</v>
+        <v>24.44312761391948</v>
       </c>
       <c r="C62">
-        <v>61.85144456366932</v>
+        <v>59.4971444293821</v>
+      </c>
+      <c r="D62">
+        <v>21.03342681607812</v>
+      </c>
+      <c r="E62">
+        <v>4.093802920775684</v>
+      </c>
+      <c r="F62">
+        <v>23.35484486969754</v>
+      </c>
+      <c r="G62">
+        <v>11.13708890378883</v>
       </c>
     </row>
     <row r="63">
@@ -1174,10 +1926,22 @@
         </is>
       </c>
       <c r="B63">
-        <v>30.54356457535861</v>
+        <v>33.96994636235697</v>
       </c>
       <c r="C63">
-        <v>55.97436278446095</v>
+        <v>51.28483555903643</v>
+      </c>
+      <c r="D63">
+        <v>25.26432208380859</v>
+      </c>
+      <c r="E63">
+        <v>3.939226959772484</v>
+      </c>
+      <c r="F63">
+        <v>33.30324767171148</v>
+      </c>
+      <c r="G63">
+        <v>10.14005216614809</v>
       </c>
     </row>
     <row r="64">
@@ -1187,10 +1951,22 @@
         </is>
       </c>
       <c r="B64">
-        <v>38.45270247903084</v>
+        <v>27.48489899065103</v>
       </c>
       <c r="C64">
-        <v>48.58048683451567</v>
+        <v>42.40804964965919</v>
+      </c>
+      <c r="D64">
+        <v>23.66249212548351</v>
+      </c>
+      <c r="E64">
+        <v>3.853149965892848</v>
+      </c>
+      <c r="F64">
+        <v>26.52083140086145</v>
+      </c>
+      <c r="G64">
+        <v>11.34279963610427</v>
       </c>
     </row>
     <row r="65">
@@ -1200,10 +1976,22 @@
         </is>
       </c>
       <c r="B65">
-        <v>27.65197192219207</v>
+        <v>32.88406941694478</v>
       </c>
       <c r="C65">
-        <v>47.05753445346371</v>
+        <v>57.86991667503607</v>
+      </c>
+      <c r="D65">
+        <v>20.79437175674648</v>
+      </c>
+      <c r="E65">
+        <v>3.738075089163342</v>
+      </c>
+      <c r="F65">
+        <v>31.88406975435858</v>
+      </c>
+      <c r="G65">
+        <v>11.64139837759779</v>
       </c>
     </row>
     <row r="66">
@@ -1213,10 +2001,22 @@
         </is>
       </c>
       <c r="B66">
-        <v>35.92134973855497</v>
+        <v>11.841861247798</v>
       </c>
       <c r="C66">
-        <v>63.52986109742753</v>
+        <v>71.84907950040142</v>
+      </c>
+      <c r="D66">
+        <v>21.62291099534539</v>
+      </c>
+      <c r="E66">
+        <v>4.085795212239907</v>
+      </c>
+      <c r="F66">
+        <v>10.8980974621986</v>
+      </c>
+      <c r="G66">
+        <v>11.31533751544361</v>
       </c>
     </row>
     <row r="67">
@@ -1226,10 +2026,22 @@
         </is>
       </c>
       <c r="B67">
-        <v>36.64727825245755</v>
+        <v>36.89242991718443</v>
       </c>
       <c r="C67">
-        <v>54.207932681377</v>
+        <v>55.40983297755563</v>
+      </c>
+      <c r="D67">
+        <v>23.50349581824113</v>
+      </c>
+      <c r="E67">
+        <v>3.709566734052332</v>
+      </c>
+      <c r="F67">
+        <v>36.01851844820797</v>
+      </c>
+      <c r="G67">
+        <v>11.80830928329974</v>
       </c>
     </row>
     <row r="68">
@@ -1239,10 +2051,22 @@
         </is>
       </c>
       <c r="B68">
-        <v>45.64934231177738</v>
+        <v>34.52429568527286</v>
       </c>
       <c r="C68">
-        <v>53.04636399853732</v>
+        <v>49.46614418930154</v>
+      </c>
+      <c r="D68">
+        <v>21.41043788496013</v>
+      </c>
+      <c r="E68">
+        <v>4.072152643826653</v>
+      </c>
+      <c r="F68">
+        <v>33.24313690301813</v>
+      </c>
+      <c r="G68">
+        <v>11.77256202521897</v>
       </c>
     </row>
     <row r="69">
@@ -1252,10 +2076,22 @@
         </is>
       </c>
       <c r="B69">
-        <v>26.03764365381159</v>
+        <v>38.6746289521377</v>
       </c>
       <c r="C69">
-        <v>50.27648560828425</v>
+        <v>48.81124026935666</v>
+      </c>
+      <c r="D69">
+        <v>23.25326214579042</v>
+      </c>
+      <c r="E69">
+        <v>4.12185560269546</v>
+      </c>
+      <c r="F69">
+        <v>37.8521740917319</v>
+      </c>
+      <c r="G69">
+        <v>13.54516678733943</v>
       </c>
     </row>
     <row r="70">
@@ -1265,10 +2101,22 @@
         </is>
       </c>
       <c r="B70">
-        <v>41.10510133563356</v>
+        <v>17.22945050390411</v>
       </c>
       <c r="C70">
-        <v>51.25099910072521</v>
+        <v>62.44054665837711</v>
+      </c>
+      <c r="D70">
+        <v>24.1648212916414</v>
+      </c>
+      <c r="E70">
+        <v>3.870772864314554</v>
+      </c>
+      <c r="F70">
+        <v>16.25682145862386</v>
+      </c>
+      <c r="G70">
+        <v>10.71655701129888</v>
       </c>
     </row>
     <row r="71">
@@ -1278,10 +2126,22 @@
         </is>
       </c>
       <c r="B71">
-        <v>27.17477760540952</v>
+        <v>36.88912815685284</v>
       </c>
       <c r="C71">
-        <v>63.95219205909981</v>
+        <v>56.14847272026265</v>
+      </c>
+      <c r="D71">
+        <v>23.18925163787053</v>
+      </c>
+      <c r="E71">
+        <v>4.061825715041915</v>
+      </c>
+      <c r="F71">
+        <v>35.81210446547169</v>
+      </c>
+      <c r="G71">
+        <v>12.07291083627389</v>
       </c>
     </row>
     <row r="72">
@@ -1291,10 +2151,22 @@
         </is>
       </c>
       <c r="B72">
-        <v>26.68254666783005</v>
+        <v>29.74403985236517</v>
       </c>
       <c r="C72">
-        <v>50.72617110877252</v>
+        <v>59.69137839214462</v>
+      </c>
+      <c r="D72">
+        <v>22.97524193615233</v>
+      </c>
+      <c r="E72">
+        <v>3.924786545936837</v>
+      </c>
+      <c r="F72">
+        <v>28.91431442524515</v>
+      </c>
+      <c r="G72">
+        <v>13.4002277584117</v>
       </c>
     </row>
     <row r="73">
@@ -1304,10 +2176,22 @@
         </is>
       </c>
       <c r="B73">
-        <v>43.69561234461192</v>
+        <v>39.29825835438068</v>
       </c>
       <c r="C73">
-        <v>50.66302976774474</v>
+        <v>54.16529224252875</v>
+      </c>
+      <c r="D73">
+        <v>22.42911851750795</v>
+      </c>
+      <c r="E73">
+        <v>3.929198749165137</v>
+      </c>
+      <c r="F73">
+        <v>38.57289680406889</v>
+      </c>
+      <c r="G73">
+        <v>12.03889528660954</v>
       </c>
     </row>
     <row r="74">
@@ -1317,10 +2201,22 @@
         </is>
       </c>
       <c r="B74">
-        <v>16.72347765800452</v>
+        <v>20.55224653262979</v>
       </c>
       <c r="C74">
-        <v>64.95322738020452</v>
+        <v>45.9455820861947</v>
+      </c>
+      <c r="D74">
+        <v>23.37943544624731</v>
+      </c>
+      <c r="E74">
+        <v>4.32250744627932</v>
+      </c>
+      <c r="F74">
+        <v>19.6258485143985</v>
+      </c>
+      <c r="G74">
+        <v>11.21476768337771</v>
       </c>
     </row>
     <row r="75">
@@ -1330,10 +2226,22 @@
         </is>
       </c>
       <c r="B75">
-        <v>22.21631637802142</v>
+        <v>43.77458002092406</v>
       </c>
       <c r="C75">
-        <v>41.33129730044993</v>
+        <v>58.64084695428735</v>
+      </c>
+      <c r="D75">
+        <v>26.69945569430335</v>
+      </c>
+      <c r="E75">
+        <v>4.027516756708843</v>
+      </c>
+      <c r="F75">
+        <v>42.82056368309154</v>
+      </c>
+      <c r="G75">
+        <v>11.56168663211563</v>
       </c>
     </row>
     <row r="76">
@@ -1343,10 +2251,22 @@
         </is>
       </c>
       <c r="B76">
-        <v>33.37408202201946</v>
+        <v>28.26350386806784</v>
       </c>
       <c r="C76">
-        <v>64.92068541667396</v>
+        <v>67.16901873391218</v>
+      </c>
+      <c r="D76">
+        <v>21.53147222126407</v>
+      </c>
+      <c r="E76">
+        <v>3.961587577537049</v>
+      </c>
+      <c r="F76">
+        <v>27.15236869210892</v>
+      </c>
+      <c r="G76">
+        <v>11.54896038578422</v>
       </c>
     </row>
     <row r="77">
@@ -1356,10 +2276,22 @@
         </is>
       </c>
       <c r="B77">
-        <v>42.97156075117927</v>
+        <v>40.07370790454397</v>
       </c>
       <c r="C77">
-        <v>61.13196065398344</v>
+        <v>45.88949061932695</v>
+      </c>
+      <c r="D77">
+        <v>23.05799261564153</v>
+      </c>
+      <c r="E77">
+        <v>4.121267236593373</v>
+      </c>
+      <c r="F77">
+        <v>39.15334457476879</v>
+      </c>
+      <c r="G77">
+        <v>12.05197667456741</v>
       </c>
     </row>
     <row r="78">
@@ -1369,10 +2301,22 @@
         </is>
       </c>
       <c r="B78">
-        <v>23.00548517337937</v>
+        <v>31.09297813061236</v>
       </c>
       <c r="C78">
-        <v>49.19760940409051</v>
+        <v>53.89257828488886</v>
+      </c>
+      <c r="D78">
+        <v>20.38262133550331</v>
+      </c>
+      <c r="E78">
+        <v>3.90257129261809</v>
+      </c>
+      <c r="F78">
+        <v>30.2577000825118</v>
+      </c>
+      <c r="G78">
+        <v>11.26477605342044</v>
       </c>
     </row>
     <row r="79">
@@ -1382,10 +2326,22 @@
         </is>
       </c>
       <c r="B79">
-        <v>41.87182782903243</v>
+        <v>30.8191241196866</v>
       </c>
       <c r="C79">
-        <v>58.95456975031923</v>
+        <v>51.49861435891505</v>
+      </c>
+      <c r="D79">
+        <v>24.07073839947378</v>
+      </c>
+      <c r="E79">
+        <v>4.075040171224229</v>
+      </c>
+      <c r="F79">
+        <v>29.84928325921819</v>
+      </c>
+      <c r="G79">
+        <v>11.61483319295561</v>
       </c>
     </row>
     <row r="80">
@@ -1395,10 +2351,22 @@
         </is>
       </c>
       <c r="B80">
-        <v>28.57906216000449</v>
+        <v>43.58057426786674</v>
       </c>
       <c r="C80">
-        <v>52.81542841649102</v>
+        <v>60.11004067306172</v>
+      </c>
+      <c r="D80">
+        <v>25.00032017770202</v>
+      </c>
+      <c r="E80">
+        <v>4.065914365043085</v>
+      </c>
+      <c r="F80">
+        <v>42.46980961872833</v>
+      </c>
+      <c r="G80">
+        <v>12.59444138703357</v>
       </c>
     </row>
     <row r="81">
@@ -1408,10 +2376,22 @@
         </is>
       </c>
       <c r="B81">
-        <v>29.60141276640775</v>
+        <v>37.9524511629512</v>
       </c>
       <c r="C81">
-        <v>57.36205969917724</v>
+        <v>61.83052883344936</v>
+      </c>
+      <c r="D81">
+        <v>22.85569834560433</v>
+      </c>
+      <c r="E81">
+        <v>4.202962062580246</v>
+      </c>
+      <c r="F81">
+        <v>36.9133189295381</v>
+      </c>
+      <c r="G81">
+        <v>13.69513886458168</v>
       </c>
     </row>
     <row r="82">
@@ -1421,10 +2401,22 @@
         </is>
       </c>
       <c r="B82">
-        <v>28.09413298692834</v>
+        <v>26.07735039475698</v>
       </c>
       <c r="C82">
-        <v>56.83943184798578</v>
+        <v>49.40994549111949</v>
+      </c>
+      <c r="D82">
+        <v>24.24521937136559</v>
+      </c>
+      <c r="E82">
+        <v>3.995645872175389</v>
+      </c>
+      <c r="F82">
+        <v>24.91238009362084</v>
+      </c>
+      <c r="G82">
+        <v>13.2155029896916</v>
       </c>
     </row>
     <row r="83">
@@ -1434,10 +2426,22 @@
         </is>
       </c>
       <c r="B83">
-        <v>26.03538952581845</v>
+        <v>32.42082230884608</v>
       </c>
       <c r="C83">
-        <v>56.48360761741624</v>
+        <v>43.28334028417983</v>
+      </c>
+      <c r="D83">
+        <v>20.72734758968685</v>
+      </c>
+      <c r="E83">
+        <v>4.019270866120972</v>
+      </c>
+      <c r="F83">
+        <v>31.35860295706418</v>
+      </c>
+      <c r="G83">
+        <v>12.55527495148966</v>
       </c>
     </row>
     <row r="84">
@@ -1447,10 +2451,22 @@
         </is>
       </c>
       <c r="B84">
-        <v>51.49650795571695</v>
+        <v>49.27667824296452</v>
       </c>
       <c r="C84">
-        <v>58.81901975943826</v>
+        <v>62.12935904742693</v>
+      </c>
+      <c r="D84">
+        <v>22.24648288050463</v>
+      </c>
+      <c r="E84">
+        <v>3.969410694158297</v>
+      </c>
+      <c r="F84">
+        <v>48.43739117919599</v>
+      </c>
+      <c r="G84">
+        <v>10.68471134007095</v>
       </c>
     </row>
     <row r="85">
@@ -1460,10 +2476,22 @@
         </is>
       </c>
       <c r="B85">
-        <v>33.24833780221655</v>
+        <v>22.56247539779152</v>
       </c>
       <c r="C85">
-        <v>56.8545665299476</v>
+        <v>60.14046238056851</v>
+      </c>
+      <c r="D85">
+        <v>23.55976579827173</v>
+      </c>
+      <c r="E85">
+        <v>4.166106110776272</v>
+      </c>
+      <c r="F85">
+        <v>21.64918652989228</v>
+      </c>
+      <c r="G85">
+        <v>10.62518792001458</v>
       </c>
     </row>
     <row r="86">
@@ -1473,10 +2501,22 @@
         </is>
       </c>
       <c r="B86">
-        <v>31.49546509071669</v>
+        <v>40.25505027247253</v>
       </c>
       <c r="C86">
-        <v>44.33532401361653</v>
+        <v>65.07405013853324</v>
+      </c>
+      <c r="D86">
+        <v>22.2565183271043</v>
+      </c>
+      <c r="E86">
+        <v>4.165556063188609</v>
+      </c>
+      <c r="F86">
+        <v>39.53459561061807</v>
+      </c>
+      <c r="G86">
+        <v>12.90465010323124</v>
       </c>
     </row>
     <row r="87">
@@ -1486,10 +2526,22 @@
         </is>
       </c>
       <c r="B87">
-        <v>31.71673738907153</v>
+        <v>44.05275281134352</v>
       </c>
       <c r="C87">
-        <v>61.67124254758173</v>
+        <v>54.94704682179785</v>
+      </c>
+      <c r="D87">
+        <v>23.88855575148531</v>
+      </c>
+      <c r="E87">
+        <v>3.786829645456456</v>
+      </c>
+      <c r="F87">
+        <v>42.92238259858833</v>
+      </c>
+      <c r="G87">
+        <v>11.84273331301842</v>
       </c>
     </row>
     <row r="88">
@@ -1499,10 +2551,22 @@
         </is>
       </c>
       <c r="B88">
-        <v>49.9789482512542</v>
+        <v>27.5135723282962</v>
       </c>
       <c r="C88">
-        <v>46.7301844091234</v>
+        <v>51.64251842114284</v>
+      </c>
+      <c r="D88">
+        <v>23.53717714877672</v>
+      </c>
+      <c r="E88">
+        <v>3.891603548789049</v>
+      </c>
+      <c r="F88">
+        <v>26.42154491985672</v>
+      </c>
+      <c r="G88">
+        <v>11.74653771751581</v>
       </c>
     </row>
     <row r="89">
@@ -1512,10 +2576,22 @@
         </is>
       </c>
       <c r="B89">
-        <v>32.56181175061567</v>
+        <v>37.71565113477804</v>
       </c>
       <c r="C89">
-        <v>56.85887497952505</v>
+        <v>56.3411961712077</v>
+      </c>
+      <c r="D89">
+        <v>25.35637251204985</v>
+      </c>
+      <c r="E89">
+        <v>4.30192479429853</v>
+      </c>
+      <c r="F89">
+        <v>36.7914666015887</v>
+      </c>
+      <c r="G89">
+        <v>11.41464543183513</v>
       </c>
     </row>
     <row r="90">
@@ -1525,10 +2601,22 @@
         </is>
       </c>
       <c r="B90">
-        <v>33.49934080230319</v>
+        <v>29.29734301709083</v>
       </c>
       <c r="C90">
-        <v>65.33101536874906</v>
+        <v>51.90839093194619</v>
+      </c>
+      <c r="D90">
+        <v>26.5357228401576</v>
+      </c>
+      <c r="E90">
+        <v>4.023786666655566</v>
+      </c>
+      <c r="F90">
+        <v>28.35949190548146</v>
+      </c>
+      <c r="G90">
+        <v>10.94866335771729</v>
       </c>
     </row>
     <row r="91">
@@ -1538,10 +2626,22 @@
         </is>
       </c>
       <c r="B91">
-        <v>31.02518852774577</v>
+        <v>45.21208844419059</v>
       </c>
       <c r="C91">
-        <v>58.43836852778984</v>
+        <v>36.09307894953973</v>
+      </c>
+      <c r="D91">
+        <v>25.42277090231746</v>
+      </c>
+      <c r="E91">
+        <v>3.952127872489295</v>
+      </c>
+      <c r="F91">
+        <v>44.4988057441714</v>
+      </c>
+      <c r="G91">
+        <v>10.45117752804703</v>
       </c>
     </row>
     <row r="92">
@@ -1551,10 +2651,22 @@
         </is>
       </c>
       <c r="B92">
-        <v>35.80941971901475</v>
+        <v>22.63393015784863</v>
       </c>
       <c r="C92">
-        <v>52.07232239584449</v>
+        <v>58.48124261897848</v>
+      </c>
+      <c r="D92">
+        <v>20.48355516567863</v>
+      </c>
+      <c r="E92">
+        <v>4.03401569360537</v>
+      </c>
+      <c r="F92">
+        <v>21.48543644859873</v>
+      </c>
+      <c r="G92">
+        <v>11.72494373689383</v>
       </c>
     </row>
     <row r="93">
@@ -1564,10 +2676,22 @@
         </is>
       </c>
       <c r="B93">
-        <v>53.59830450669628</v>
+        <v>41.77871693956116</v>
       </c>
       <c r="C93">
-        <v>46.20444404212178</v>
+        <v>47.77038147820075</v>
+      </c>
+      <c r="D93">
+        <v>25.17314629319394</v>
+      </c>
+      <c r="E93">
+        <v>4.110589703461608</v>
+      </c>
+      <c r="F93">
+        <v>40.38246468849851</v>
+      </c>
+      <c r="G93">
+        <v>11.02507170062177</v>
       </c>
     </row>
     <row r="94">
@@ -1577,10 +2701,22 @@
         </is>
       </c>
       <c r="B94">
-        <v>41.20020878147511</v>
+        <v>34.69601892439146</v>
       </c>
       <c r="C94">
-        <v>52.01893754828187</v>
+        <v>54.66067941013287</v>
+      </c>
+      <c r="D94">
+        <v>26.10693695294588</v>
+      </c>
+      <c r="E94">
+        <v>4.231813353464654</v>
+      </c>
+      <c r="F94">
+        <v>33.63910032094179</v>
+      </c>
+      <c r="G94">
+        <v>9.683799278530397</v>
       </c>
     </row>
     <row r="95">
@@ -1590,10 +2726,22 @@
         </is>
       </c>
       <c r="B95">
-        <v>34.97525010487074</v>
+        <v>43.97951469826275</v>
       </c>
       <c r="C95">
-        <v>50.641626709881</v>
+        <v>45.44502182438195</v>
+      </c>
+      <c r="D95">
+        <v>20.39676434279703</v>
+      </c>
+      <c r="E95">
+        <v>3.90995098190847</v>
+      </c>
+      <c r="F95">
+        <v>42.98829440331416</v>
+      </c>
+      <c r="G95">
+        <v>10.97744627786963</v>
       </c>
     </row>
     <row r="96">
@@ -1603,10 +2751,22 @@
         </is>
       </c>
       <c r="B96">
-        <v>43.80540314289258</v>
+        <v>32.26031409496475</v>
       </c>
       <c r="C96">
-        <v>59.71406330504946</v>
+        <v>59.80185270946399</v>
+      </c>
+      <c r="D96">
+        <v>20.2070774281246</v>
+      </c>
+      <c r="E96">
+        <v>4.311496370567833</v>
+      </c>
+      <c r="F96">
+        <v>31.38069684125321</v>
+      </c>
+      <c r="G96">
+        <v>13.56334317453702</v>
       </c>
     </row>
     <row r="97">
@@ -1616,10 +2776,22 @@
         </is>
       </c>
       <c r="B97">
-        <v>30.62566156890932</v>
+        <v>23.73510382571141</v>
       </c>
       <c r="C97">
-        <v>58.92323236827756</v>
+        <v>49.32695172724448</v>
+      </c>
+      <c r="D97">
+        <v>23.48549162446884</v>
+      </c>
+      <c r="E97">
+        <v>4.060459279307445</v>
+      </c>
+      <c r="F97">
+        <v>22.85104148693994</v>
+      </c>
+      <c r="G97">
+        <v>12.54426569891784</v>
       </c>
     </row>
     <row r="98">
@@ -1629,10 +2801,22 @@
         </is>
       </c>
       <c r="B98">
-        <v>39.28334384418911</v>
+        <v>32.854121872055</v>
       </c>
       <c r="C98">
-        <v>51.5787951712523</v>
+        <v>67.04746809534912</v>
+      </c>
+      <c r="D98">
+        <v>21.63988236858926</v>
+      </c>
+      <c r="E98">
+        <v>4.234181115912361</v>
+      </c>
+      <c r="F98">
+        <v>32.21974016407884</v>
+      </c>
+      <c r="G98">
+        <v>12.27249559636813</v>
       </c>
     </row>
     <row r="99">
@@ -1642,10 +2826,22 @@
         </is>
       </c>
       <c r="B99">
-        <v>24.97772531572208</v>
+        <v>33.27925770161179</v>
       </c>
       <c r="C99">
-        <v>71.76719915658789</v>
+        <v>48.10038734933763</v>
+      </c>
+      <c r="D99">
+        <v>24.08829397733289</v>
+      </c>
+      <c r="E99">
+        <v>4.116243567510098</v>
+      </c>
+      <c r="F99">
+        <v>32.33044106848471</v>
+      </c>
+      <c r="G99">
+        <v>10.91428661220003</v>
       </c>
     </row>
     <row r="100">
@@ -1655,10 +2851,22 @@
         </is>
       </c>
       <c r="B100">
-        <v>33.83641386419566</v>
+        <v>26.79758841971452</v>
       </c>
       <c r="C100">
-        <v>47.67923316869067</v>
+        <v>70.51340724828731</v>
+      </c>
+      <c r="D100">
+        <v>22.43498496822279</v>
+      </c>
+      <c r="E100">
+        <v>4.050532187133506</v>
+      </c>
+      <c r="F100">
+        <v>26.13884795657924</v>
+      </c>
+      <c r="G100">
+        <v>11.48942019102744</v>
       </c>
     </row>
     <row r="101">
@@ -1668,10 +2876,22 @@
         </is>
       </c>
       <c r="B101">
-        <v>38.7847750526428</v>
+        <v>20.3598936023994</v>
       </c>
       <c r="C101">
-        <v>59.44117605231041</v>
+        <v>63.10547042308737</v>
+      </c>
+      <c r="D101">
+        <v>23.56022705714587</v>
+      </c>
+      <c r="E101">
+        <v>3.617040782860569</v>
+      </c>
+      <c r="F101">
+        <v>19.56753017380564</v>
+      </c>
+      <c r="G101">
+        <v>12.31241734192292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>